<commit_message>
Added 3 songs, fixed visibility
</commit_message>
<xml_diff>
--- a/tables/covers.xlsx
+++ b/tables/covers.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="covers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="300">
   <si>
     <t>num</t>
   </si>
@@ -896,6 +896,24 @@
   </si>
   <si>
     <t>Harvest Moon</t>
+  </si>
+  <si>
+    <t>Maroon 5 (Pentatonix</t>
+  </si>
+  <si>
+    <t>Moves Like Jagger</t>
+  </si>
+  <si>
+    <t>Dua Lipa (Pentatonix)</t>
+  </si>
+  <si>
+    <t>Break My Heart</t>
+  </si>
+  <si>
+    <t>Demi Levato (Pentatonix)</t>
+  </si>
+  <si>
+    <t>Sorry Not Sorry</t>
   </si>
 </sst>
 </file>
@@ -1724,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3444,6 +3462,39 @@
         <v>293</v>
       </c>
     </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>294</v>
+      </c>
+      <c r="C151" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A152">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>296</v>
+      </c>
+      <c r="C152" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A153">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>298</v>
+      </c>
+      <c r="C153" t="s">
+        <v>299</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>